<commit_message>
Images and sounds data updated
</commit_message>
<xml_diff>
--- a/images_data.xlsx
+++ b/images_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4303" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="81">
   <si>
     <t>Timestamp</t>
   </si>
@@ -25416,6 +25416,128 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="205">
+      <c r="A205" s="2">
+        <v>43847.691497569445</v>
+      </c>
+      <c r="B205" s="3">
+        <v>13.0</v>
+      </c>
+      <c r="C205" s="4">
+        <v>43.0</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E205" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F205" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G205" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H205" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I205" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J205" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="K205" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L205" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="M205" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N205" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="O205" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P205" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="Q205" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R205" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="S205" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="T205" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="U205" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="V205" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="W205" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X205" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="Y205" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z205" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="AA205" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB205" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="AC205" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD205" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="AE205" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF205" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AG205" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH205" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="AI205" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ205" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="AK205" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL205" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="AM205" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN205" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>